<commit_message>
Corrección motores M101AP Escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion02/Escaleta_LE_10_02_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion02/Escaleta_LE_10_02_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Lenguaje\fuentes\contenidos\grado10\guion02\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-181" yWindow="204" windowWidth="25603" windowHeight="13902"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14000"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,20 +13,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$U$51</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="320">
   <si>
     <t>Asignatura</t>
   </si>
@@ -437,9 +432,6 @@
   </si>
   <si>
     <t xml:space="preserve">(DBA: 5) Diseñar cinco (5) oraciones metafóricas y cinco (5) no metafóricas o simples, para que el estudiante las arrastre en dos contenedores diferentes (Metáforas y No metáforas, por ejemplo). </t>
-  </si>
-  <si>
-    <t>Recurso M101AP-01</t>
   </si>
   <si>
     <t xml:space="preserve">Actividad diagnóstica con base en la lectura sobre el conversatorio </t>
@@ -1273,6 +1265,12 @@
   </si>
   <si>
     <t>(DBA: 4) Es importante que al menos parte de esta información haya sido presentada en el Interactivo de la sección. Varias lenguas (indígenas, el criol; incluso el inglés como lenguaje en San Andrés, en fin) serán ubicadas por el estudiante en contenedores que las clasifiquen, o bien por la regíon en la que se hablan, la etnia u otra.</t>
+  </si>
+  <si>
+    <t>Recurso M101A-05</t>
+  </si>
+  <si>
+    <t>Recurso M101A-06</t>
   </si>
 </sst>
 </file>
@@ -2282,7 +2280,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2290,33 +2288,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.46484375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.19921875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="24.265625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="24.33203125" style="12" customWidth="1"/>
     <col min="7" max="7" width="41.33203125" style="12" customWidth="1"/>
-    <col min="8" max="9" width="4.53125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="4.5" style="2" customWidth="1"/>
     <col min="10" max="10" width="65.6640625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="8.86328125" style="48" customWidth="1"/>
-    <col min="12" max="12" width="11.19921875" style="48" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="48" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" style="48" customWidth="1"/>
     <col min="13" max="13" width="6" style="48" customWidth="1"/>
     <col min="14" max="14" width="6" style="12" customWidth="1"/>
     <col min="15" max="15" width="60" style="12" customWidth="1"/>
-    <col min="16" max="16" width="7.265625" style="2" customWidth="1"/>
-    <col min="17" max="21" width="13.19921875" style="12" customWidth="1"/>
-    <col min="22" max="16384" width="10.6640625" style="12"/>
+    <col min="16" max="16" width="7.33203125" style="2" customWidth="1"/>
+    <col min="17" max="21" width="13.1640625" style="12" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" ht="15" thickBot="1">
       <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
@@ -2379,7 +2377,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="14" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:21" s="14" customFormat="1" ht="15" thickBot="1">
       <c r="A2" s="50"/>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -2406,7 +2404,7 @@
       <c r="T2" s="50"/>
       <c r="U2" s="50"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21">
       <c r="A3" s="15" t="s">
         <v>68</v>
       </c>
@@ -2465,7 +2463,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21">
       <c r="A4" s="15" t="s">
         <v>68</v>
       </c>
@@ -2524,7 +2522,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21">
       <c r="A5" s="15" t="s">
         <v>68</v>
       </c>
@@ -2583,7 +2581,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21">
       <c r="A6" s="15" t="s">
         <v>68</v>
       </c>
@@ -2599,7 +2597,7 @@
       <c r="E6" s="26"/>
       <c r="F6" s="27"/>
       <c r="G6" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H6" s="10">
         <v>4</v>
@@ -2608,7 +2606,7 @@
         <v>108</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K6" s="31" t="s">
         <v>69</v>
@@ -2617,11 +2615,11 @@
         <v>32</v>
       </c>
       <c r="M6" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N6" s="23"/>
       <c r="O6" s="30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>19</v>
@@ -2636,13 +2634,13 @@
         <v>102</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>119</v>
+        <v>319</v>
       </c>
       <c r="U6" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21">
       <c r="A7" s="15" t="s">
         <v>68</v>
       </c>
@@ -2658,7 +2656,7 @@
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
       <c r="G7" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H7" s="10">
         <v>5</v>
@@ -2667,7 +2665,7 @@
         <v>108</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K7" s="31" t="s">
         <v>69</v>
@@ -2680,7 +2678,7 @@
       </c>
       <c r="N7" s="23"/>
       <c r="O7" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P7" s="11" t="s">
         <v>19</v>
@@ -2695,13 +2693,13 @@
         <v>102</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U7" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21">
       <c r="A8" s="15" t="s">
         <v>68</v>
       </c>
@@ -2717,7 +2715,7 @@
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
       <c r="G8" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H8" s="10">
         <v>6</v>
@@ -2726,7 +2724,7 @@
         <v>108</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K8" s="31" t="s">
         <v>69</v>
@@ -2739,7 +2737,7 @@
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P8" s="11" t="s">
         <v>19</v>
@@ -2754,13 +2752,13 @@
         <v>102</v>
       </c>
       <c r="T8" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U8" s="25" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21">
       <c r="A9" s="15" t="s">
         <v>68</v>
       </c>
@@ -2798,7 +2796,7 @@
       <c r="M9" s="23"/>
       <c r="N9" s="23"/>
       <c r="O9" s="30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P9" s="11" t="s">
         <v>19</v>
@@ -2819,7 +2817,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21">
       <c r="A10" s="15" t="s">
         <v>68</v>
       </c>
@@ -2836,10 +2834,10 @@
         <v>100</v>
       </c>
       <c r="F10" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="G10" s="28" t="s">
         <v>157</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>158</v>
       </c>
       <c r="H10" s="10">
         <v>8</v>
@@ -2848,7 +2846,7 @@
         <v>108</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K10" s="31" t="s">
         <v>70</v>
@@ -2859,7 +2857,7 @@
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
       <c r="O10" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P10" s="11" t="s">
         <v>19</v>
@@ -2874,13 +2872,13 @@
         <v>105</v>
       </c>
       <c r="T10" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U10" s="25" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21">
       <c r="A11" s="15" t="s">
         <v>68</v>
       </c>
@@ -2897,10 +2895,10 @@
         <v>100</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H11" s="10">
         <v>9</v>
@@ -2909,7 +2907,7 @@
         <v>108</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="31" t="s">
         <v>69</v>
@@ -2922,7 +2920,7 @@
       </c>
       <c r="N11" s="23"/>
       <c r="O11" s="39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P11" s="11" t="s">
         <v>19</v>
@@ -2937,13 +2935,13 @@
         <v>102</v>
       </c>
       <c r="T11" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="U11" s="25" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21">
       <c r="A12" s="15" t="s">
         <v>68</v>
       </c>
@@ -2960,10 +2958,10 @@
         <v>100</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H12" s="10">
         <v>10</v>
@@ -2972,18 +2970,18 @@
         <v>94</v>
       </c>
       <c r="J12" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K12" s="31" t="s">
         <v>70</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
       <c r="O12" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>19</v>
@@ -2998,13 +2996,13 @@
         <v>105</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U12" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21">
       <c r="A13" s="15" t="s">
         <v>68</v>
       </c>
@@ -3018,13 +3016,13 @@
         <v>99</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H13" s="10">
         <v>11</v>
@@ -3033,7 +3031,7 @@
         <v>94</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K13" s="31" t="s">
         <v>70</v>
@@ -3044,7 +3042,7 @@
       <c r="M13" s="23"/>
       <c r="N13" s="23"/>
       <c r="O13" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P13" s="11" t="s">
         <v>19</v>
@@ -3059,13 +3057,13 @@
         <v>105</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="U13" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21">
       <c r="A14" s="15" t="s">
         <v>68</v>
       </c>
@@ -3079,13 +3077,13 @@
         <v>99</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H14" s="10">
         <v>12</v>
@@ -3094,7 +3092,7 @@
         <v>94</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K14" s="31" t="s">
         <v>70</v>
@@ -3105,7 +3103,7 @@
       <c r="M14" s="23"/>
       <c r="N14" s="23"/>
       <c r="O14" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>19</v>
@@ -3120,13 +3118,13 @@
         <v>105</v>
       </c>
       <c r="T14" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U14" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21">
       <c r="A15" s="15" t="s">
         <v>68</v>
       </c>
@@ -3140,13 +3138,13 @@
         <v>99</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H15" s="10">
         <v>13</v>
@@ -3155,7 +3153,7 @@
         <v>108</v>
       </c>
       <c r="J15" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K15" s="31" t="s">
         <v>70</v>
@@ -3166,7 +3164,7 @@
       <c r="M15" s="23"/>
       <c r="N15" s="23"/>
       <c r="O15" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>19</v>
@@ -3181,13 +3179,13 @@
         <v>105</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U15" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21">
       <c r="A16" s="15" t="s">
         <v>68</v>
       </c>
@@ -3201,13 +3199,13 @@
         <v>99</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H16" s="10">
         <v>14</v>
@@ -3216,7 +3214,7 @@
         <v>94</v>
       </c>
       <c r="J16" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K16" s="31" t="s">
         <v>70</v>
@@ -3227,7 +3225,7 @@
       <c r="M16" s="23"/>
       <c r="N16" s="23"/>
       <c r="O16" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>19</v>
@@ -3242,13 +3240,13 @@
         <v>105</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U16" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21">
       <c r="A17" s="15" t="s">
         <v>68</v>
       </c>
@@ -3262,13 +3260,13 @@
         <v>99</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F17" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="G17" s="28" t="s">
         <v>147</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>148</v>
       </c>
       <c r="H17" s="10">
         <v>15</v>
@@ -3277,18 +3275,18 @@
         <v>94</v>
       </c>
       <c r="J17" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K17" s="31" t="s">
         <v>70</v>
       </c>
       <c r="L17" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M17" s="23"/>
       <c r="N17" s="23"/>
       <c r="O17" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>19</v>
@@ -3303,13 +3301,13 @@
         <v>105</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U17" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21">
       <c r="A18" s="15" t="s">
         <v>68</v>
       </c>
@@ -3323,13 +3321,13 @@
         <v>99</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H18" s="10">
         <v>16</v>
@@ -3338,7 +3336,7 @@
         <v>108</v>
       </c>
       <c r="J18" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K18" s="31" t="s">
         <v>70</v>
@@ -3349,7 +3347,7 @@
       <c r="M18" s="23"/>
       <c r="N18" s="23"/>
       <c r="O18" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P18" s="11" t="s">
         <v>19</v>
@@ -3364,13 +3362,13 @@
         <v>105</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="U18" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21">
       <c r="A19" s="15" t="s">
         <v>68</v>
       </c>
@@ -3384,13 +3382,13 @@
         <v>99</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H19" s="10">
         <v>17</v>
@@ -3399,7 +3397,7 @@
         <v>108</v>
       </c>
       <c r="J19" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K19" s="31" t="s">
         <v>70</v>
@@ -3410,7 +3408,7 @@
       <c r="M19" s="23"/>
       <c r="N19" s="23"/>
       <c r="O19" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P19" s="11" t="s">
         <v>19</v>
@@ -3425,13 +3423,13 @@
         <v>105</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U19" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21">
       <c r="A20" s="15" t="s">
         <v>68</v>
       </c>
@@ -3445,11 +3443,11 @@
         <v>99</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F20" s="27"/>
       <c r="G20" s="28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H20" s="10">
         <v>18</v>
@@ -3458,7 +3456,7 @@
         <v>94</v>
       </c>
       <c r="J20" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K20" s="31" t="s">
         <v>70</v>
@@ -3469,7 +3467,7 @@
       <c r="M20" s="23"/>
       <c r="N20" s="23"/>
       <c r="O20" s="30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P20" s="11" t="s">
         <v>19</v>
@@ -3484,13 +3482,13 @@
         <v>105</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U20" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21">
       <c r="A21" s="15" t="s">
         <v>68</v>
       </c>
@@ -3504,11 +3502,11 @@
         <v>99</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F21" s="27"/>
       <c r="G21" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H21" s="10">
         <v>19</v>
@@ -3517,7 +3515,7 @@
         <v>108</v>
       </c>
       <c r="J21" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K21" s="31" t="s">
         <v>70</v>
@@ -3528,7 +3526,7 @@
       <c r="M21" s="23"/>
       <c r="N21" s="23"/>
       <c r="O21" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P21" s="11" t="s">
         <v>19</v>
@@ -3543,13 +3541,13 @@
         <v>105</v>
       </c>
       <c r="T21" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="U21" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21">
       <c r="A22" s="15" t="s">
         <v>68</v>
       </c>
@@ -3563,11 +3561,11 @@
         <v>99</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H22" s="10">
         <v>20</v>
@@ -3576,7 +3574,7 @@
         <v>108</v>
       </c>
       <c r="J22" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K22" s="31" t="s">
         <v>70</v>
@@ -3587,7 +3585,7 @@
       <c r="M22" s="23"/>
       <c r="N22" s="23"/>
       <c r="O22" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P22" s="11" t="s">
         <v>20</v>
@@ -3602,13 +3600,13 @@
         <v>105</v>
       </c>
       <c r="T22" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U22" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21">
       <c r="A23" s="15" t="s">
         <v>68</v>
       </c>
@@ -3619,12 +3617,12 @@
         <v>91</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="27"/>
       <c r="G23" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H23" s="10">
         <v>21</v>
@@ -3633,7 +3631,7 @@
         <v>94</v>
       </c>
       <c r="J23" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K23" s="31" t="s">
         <v>69</v>
@@ -3646,7 +3644,7 @@
         <v>35</v>
       </c>
       <c r="O23" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P23" s="11" t="s">
         <v>19</v>
@@ -3655,19 +3653,19 @@
         <v>6</v>
       </c>
       <c r="R23" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="S23" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="S23" s="5" t="s">
+      <c r="T23" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="T23" s="5" t="s">
+      <c r="U23" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="U23" s="33" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" s="15" t="s">
         <v>68</v>
       </c>
@@ -3678,12 +3676,12 @@
         <v>91</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="27"/>
       <c r="G24" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H24" s="10">
         <v>22</v>
@@ -3692,7 +3690,7 @@
         <v>108</v>
       </c>
       <c r="J24" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K24" s="31" t="s">
         <v>69</v>
@@ -3705,7 +3703,7 @@
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P24" s="11" t="s">
         <v>19</v>
@@ -3720,13 +3718,13 @@
         <v>102</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U24" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21">
       <c r="A25" s="15" t="s">
         <v>68</v>
       </c>
@@ -3737,12 +3735,12 @@
         <v>91</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="27"/>
       <c r="G25" s="28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H25" s="10">
         <v>23</v>
@@ -3751,7 +3749,7 @@
         <v>108</v>
       </c>
       <c r="J25" s="28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K25" s="31" t="s">
         <v>70</v>
@@ -3762,28 +3760,28 @@
       <c r="M25" s="23"/>
       <c r="N25" s="23"/>
       <c r="O25" s="30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P25" s="11" t="s">
         <v>19</v>
       </c>
       <c r="Q25" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R25" s="5" t="s">
         <v>97</v>
       </c>
       <c r="S25" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="T25" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="T25" s="5" t="s">
+      <c r="U25" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="U25" s="33" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" s="15" t="s">
         <v>68</v>
       </c>
@@ -3794,14 +3792,14 @@
         <v>91</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H26" s="10">
         <v>24</v>
@@ -3810,7 +3808,7 @@
         <v>94</v>
       </c>
       <c r="J26" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K26" s="31" t="s">
         <v>70</v>
@@ -3821,28 +3819,28 @@
       <c r="M26" s="23"/>
       <c r="N26" s="23"/>
       <c r="O26" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P26" s="11" t="s">
         <v>19</v>
       </c>
       <c r="Q26" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="R26" s="5" t="s">
         <v>97</v>
       </c>
       <c r="S26" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="T26" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="T26" s="5" t="s">
+      <c r="U26" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="U26" s="33" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" s="15" t="s">
         <v>68</v>
       </c>
@@ -3853,14 +3851,14 @@
         <v>91</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F27" s="27"/>
       <c r="G27" s="28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H27" s="10">
         <v>25</v>
@@ -3869,7 +3867,7 @@
         <v>108</v>
       </c>
       <c r="J27" s="29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K27" s="31" t="s">
         <v>69</v>
@@ -3882,7 +3880,7 @@
       </c>
       <c r="N27" s="23"/>
       <c r="O27" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P27" s="11" t="s">
         <v>19</v>
@@ -3897,13 +3895,13 @@
         <v>102</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U27" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21">
       <c r="A28" s="15" t="s">
         <v>68</v>
       </c>
@@ -3914,14 +3912,14 @@
         <v>91</v>
       </c>
       <c r="D28" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F28" s="27"/>
       <c r="G28" s="28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H28" s="10">
         <v>26</v>
@@ -3930,7 +3928,7 @@
         <v>108</v>
       </c>
       <c r="J28" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K28" s="31" t="s">
         <v>69</v>
@@ -3943,7 +3941,7 @@
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P28" s="11" t="s">
         <v>19</v>
@@ -3958,13 +3956,13 @@
         <v>102</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U28" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:21">
       <c r="A29" s="15" t="s">
         <v>68</v>
       </c>
@@ -3975,14 +3973,14 @@
         <v>91</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H29" s="10">
         <v>27</v>
@@ -3991,7 +3989,7 @@
         <v>94</v>
       </c>
       <c r="J29" s="29" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K29" s="31" t="s">
         <v>69</v>
@@ -4004,7 +4002,7 @@
         <v>42</v>
       </c>
       <c r="O29" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P29" s="11" t="s">
         <v>19</v>
@@ -4013,19 +4011,19 @@
         <v>6</v>
       </c>
       <c r="R29" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="S29" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="S29" s="5" t="s">
-        <v>196</v>
-      </c>
       <c r="T29" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="U29" s="33" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" s="15" t="s">
         <v>68</v>
       </c>
@@ -4036,14 +4034,14 @@
         <v>91</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F30" s="27"/>
       <c r="G30" s="40" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H30" s="10">
         <v>28</v>
@@ -4052,7 +4050,7 @@
         <v>108</v>
       </c>
       <c r="J30" s="29" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K30" s="31" t="s">
         <v>69</v>
@@ -4065,7 +4063,7 @@
       </c>
       <c r="N30" s="23"/>
       <c r="O30" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P30" s="11" t="s">
         <v>19</v>
@@ -4080,13 +4078,13 @@
         <v>102</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="U30" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:21">
       <c r="A31" s="15" t="s">
         <v>68</v>
       </c>
@@ -4097,14 +4095,14 @@
         <v>91</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F31" s="27"/>
       <c r="G31" s="28" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H31" s="10">
         <v>29</v>
@@ -4113,7 +4111,7 @@
         <v>94</v>
       </c>
       <c r="J31" s="29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K31" s="31" t="s">
         <v>70</v>
@@ -4124,28 +4122,28 @@
       <c r="M31" s="23"/>
       <c r="N31" s="23"/>
       <c r="O31" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P31" s="11" t="s">
         <v>19</v>
       </c>
       <c r="Q31" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R31" s="5" t="s">
         <v>97</v>
       </c>
       <c r="S31" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="T31" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="T31" s="5" t="s">
+      <c r="U31" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="U31" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" s="15" t="s">
         <v>68</v>
       </c>
@@ -4156,14 +4154,14 @@
         <v>91</v>
       </c>
       <c r="D32" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F32" s="27"/>
       <c r="G32" s="28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H32" s="10">
         <v>30</v>
@@ -4172,7 +4170,7 @@
         <v>108</v>
       </c>
       <c r="J32" s="29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K32" s="31" t="s">
         <v>69</v>
@@ -4185,7 +4183,7 @@
       </c>
       <c r="N32" s="23"/>
       <c r="O32" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P32" s="11" t="s">
         <v>19</v>
@@ -4200,13 +4198,13 @@
         <v>102</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U32" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:21">
       <c r="A33" s="15" t="s">
         <v>68</v>
       </c>
@@ -4217,16 +4215,16 @@
         <v>91</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E33" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="G33" s="28" t="s">
         <v>246</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="G33" s="28" t="s">
-        <v>247</v>
       </c>
       <c r="H33" s="10">
         <v>31</v>
@@ -4235,7 +4233,7 @@
         <v>94</v>
       </c>
       <c r="J33" s="29" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K33" s="31" t="s">
         <v>70</v>
@@ -4246,28 +4244,28 @@
       <c r="M33" s="23"/>
       <c r="N33" s="23"/>
       <c r="O33" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P33" s="11" t="s">
         <v>19</v>
       </c>
       <c r="Q33" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R33" s="5" t="s">
         <v>97</v>
       </c>
       <c r="S33" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T33" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="U33" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" s="15" t="s">
         <v>68</v>
       </c>
@@ -4278,16 +4276,16 @@
         <v>91</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H34" s="10">
         <v>32</v>
@@ -4296,7 +4294,7 @@
         <v>108</v>
       </c>
       <c r="J34" s="29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K34" s="31" t="s">
         <v>69</v>
@@ -4309,7 +4307,7 @@
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P34" s="11" t="s">
         <v>19</v>
@@ -4324,13 +4322,13 @@
         <v>102</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="U34" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21">
       <c r="A35" s="15" t="s">
         <v>68</v>
       </c>
@@ -4341,14 +4339,14 @@
         <v>91</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F35" s="27"/>
       <c r="G35" s="28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H35" s="10">
         <v>33</v>
@@ -4357,7 +4355,7 @@
         <v>94</v>
       </c>
       <c r="J35" s="29" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K35" s="31" t="s">
         <v>70</v>
@@ -4368,28 +4366,28 @@
       <c r="M35" s="23"/>
       <c r="N35" s="23"/>
       <c r="O35" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P35" s="11" t="s">
         <v>19</v>
       </c>
       <c r="Q35" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R35" s="5" t="s">
         <v>97</v>
       </c>
       <c r="S35" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="U35" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" s="15" t="s">
         <v>68</v>
       </c>
@@ -4400,14 +4398,14 @@
         <v>91</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E36" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F36" s="27"/>
       <c r="G36" s="28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H36" s="10">
         <v>34</v>
@@ -4416,7 +4414,7 @@
         <v>108</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K36" s="31" t="s">
         <v>69</v>
@@ -4429,7 +4427,7 @@
       </c>
       <c r="N36" s="23"/>
       <c r="O36" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P36" s="11" t="s">
         <v>19</v>
@@ -4444,13 +4442,13 @@
         <v>102</v>
       </c>
       <c r="T36" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="U36" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:21">
       <c r="A37" s="15" t="s">
         <v>68</v>
       </c>
@@ -4461,16 +4459,16 @@
         <v>91</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F37" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="G37" s="28" t="s">
         <v>277</v>
-      </c>
-      <c r="G37" s="28" t="s">
-        <v>278</v>
       </c>
       <c r="H37" s="10">
         <v>35</v>
@@ -4479,7 +4477,7 @@
         <v>94</v>
       </c>
       <c r="J37" s="29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K37" s="31" t="s">
         <v>70</v>
@@ -4490,28 +4488,28 @@
       <c r="M37" s="23"/>
       <c r="N37" s="23"/>
       <c r="O37" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P37" s="11" t="s">
         <v>19</v>
       </c>
       <c r="Q37" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R37" s="5" t="s">
         <v>97</v>
       </c>
       <c r="S37" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T37" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="U37" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" s="15" t="s">
         <v>68</v>
       </c>
@@ -4522,16 +4520,16 @@
         <v>91</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H38" s="10">
         <v>36</v>
@@ -4540,7 +4538,7 @@
         <v>108</v>
       </c>
       <c r="J38" s="29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K38" s="31" t="s">
         <v>70</v>
@@ -4551,28 +4549,28 @@
       <c r="M38" s="23"/>
       <c r="N38" s="23"/>
       <c r="O38" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P38" s="11" t="s">
         <v>19</v>
       </c>
       <c r="Q38" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R38" s="5" t="s">
         <v>97</v>
       </c>
       <c r="S38" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T38" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="U38" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39" s="15" t="s">
         <v>68</v>
       </c>
@@ -4583,14 +4581,14 @@
         <v>91</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F39" s="27"/>
       <c r="G39" s="28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H39" s="10">
         <v>37</v>
@@ -4599,7 +4597,7 @@
         <v>108</v>
       </c>
       <c r="J39" s="29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K39" s="31" t="s">
         <v>69</v>
@@ -4610,7 +4608,7 @@
       <c r="M39" s="23"/>
       <c r="N39" s="23"/>
       <c r="O39" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P39" s="11" t="s">
         <v>19</v>
@@ -4625,13 +4623,13 @@
         <v>102</v>
       </c>
       <c r="T39" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="U39" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:21">
       <c r="A40" s="15" t="s">
         <v>68</v>
       </c>
@@ -4642,14 +4640,14 @@
         <v>91</v>
       </c>
       <c r="D40" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F40" s="27"/>
       <c r="G40" s="28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H40" s="10">
         <v>38</v>
@@ -4658,7 +4656,7 @@
         <v>108</v>
       </c>
       <c r="J40" s="29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K40" s="31" t="s">
         <v>69</v>
@@ -4671,7 +4669,7 @@
       </c>
       <c r="N40" s="23"/>
       <c r="O40" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="P40" s="11" t="s">
         <v>20</v>
@@ -4686,13 +4684,13 @@
         <v>102</v>
       </c>
       <c r="T40" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U40" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:21">
       <c r="A41" s="15" t="s">
         <v>68</v>
       </c>
@@ -4703,12 +4701,12 @@
         <v>91</v>
       </c>
       <c r="D41" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E41" s="26"/>
       <c r="F41" s="27"/>
       <c r="G41" s="29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H41" s="10">
         <v>39</v>
@@ -4717,7 +4715,7 @@
         <v>94</v>
       </c>
       <c r="J41" s="29" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K41" s="31" t="s">
         <v>69</v>
@@ -4730,7 +4728,7 @@
         <v>45</v>
       </c>
       <c r="O41" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P41" s="11" t="s">
         <v>19</v>
@@ -4739,19 +4737,19 @@
         <v>6</v>
       </c>
       <c r="R41" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="S41" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="S41" s="5" t="s">
-        <v>196</v>
-      </c>
       <c r="T41" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="U41" s="33" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" s="41" customFormat="1" x14ac:dyDescent="0.45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" s="41" customFormat="1">
       <c r="A42" s="15" t="s">
         <v>68</v>
       </c>
@@ -4762,12 +4760,12 @@
         <v>91</v>
       </c>
       <c r="D42" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E42" s="26"/>
       <c r="F42" s="27"/>
       <c r="G42" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H42" s="10">
         <v>40</v>
@@ -4776,20 +4774,20 @@
         <v>108</v>
       </c>
       <c r="J42" s="29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K42" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L42" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M42" s="23" t="s">
         <v>24</v>
       </c>
       <c r="N42" s="23"/>
       <c r="O42" s="30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P42" s="11" t="s">
         <v>19</v>
@@ -4804,13 +4802,13 @@
         <v>102</v>
       </c>
       <c r="T42" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U42" s="25" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:21">
       <c r="A43" s="15" t="s">
         <v>68</v>
       </c>
@@ -4821,14 +4819,14 @@
         <v>91</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F43" s="27"/>
       <c r="G43" s="28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H43" s="10">
         <v>41</v>
@@ -4837,20 +4835,20 @@
         <v>108</v>
       </c>
       <c r="J43" s="29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K43" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L43" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M43" s="23" t="s">
         <v>62</v>
       </c>
       <c r="N43" s="23"/>
       <c r="O43" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P43" s="11" t="s">
         <v>19</v>
@@ -4865,13 +4863,13 @@
         <v>102</v>
       </c>
       <c r="T43" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="U43" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:21">
       <c r="A44" s="15" t="s">
         <v>68</v>
       </c>
@@ -4882,14 +4880,14 @@
         <v>91</v>
       </c>
       <c r="D44" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F44" s="27"/>
       <c r="G44" s="28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H44" s="10">
         <v>42</v>
@@ -4898,20 +4896,20 @@
         <v>108</v>
       </c>
       <c r="J44" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L44" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M44" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N44" s="23"/>
       <c r="O44" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P44" s="11" t="s">
         <v>20</v>
@@ -4926,13 +4924,13 @@
         <v>102</v>
       </c>
       <c r="T44" s="5" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="U44" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:21">
       <c r="A45" s="15" t="s">
         <v>68</v>
       </c>
@@ -4943,12 +4941,12 @@
         <v>91</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E45" s="26"/>
       <c r="F45" s="27"/>
       <c r="G45" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H45" s="10">
         <v>43</v>
@@ -4957,18 +4955,18 @@
         <v>108</v>
       </c>
       <c r="J45" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K45" s="31" t="s">
         <v>70</v>
       </c>
       <c r="L45" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M45" s="23"/>
       <c r="N45" s="23"/>
       <c r="O45" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P45" s="11" t="s">
         <v>19</v>
@@ -4983,13 +4981,13 @@
         <v>105</v>
       </c>
       <c r="T45" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U45" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:21">
       <c r="A46" s="15" t="s">
         <v>68</v>
       </c>
@@ -5000,12 +4998,12 @@
         <v>91</v>
       </c>
       <c r="D46" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E46" s="42"/>
       <c r="F46" s="43"/>
       <c r="G46" s="28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H46" s="10">
         <v>44</v>
@@ -5014,18 +5012,18 @@
         <v>108</v>
       </c>
       <c r="J46" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K46" s="31" t="s">
         <v>70</v>
       </c>
       <c r="L46" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M46" s="23"/>
       <c r="N46" s="23"/>
       <c r="O46" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P46" s="11" t="s">
         <v>19</v>
@@ -5040,13 +5038,13 @@
         <v>105</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U46" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:21">
       <c r="A47" s="15" t="s">
         <v>68</v>
       </c>
@@ -5057,12 +5055,12 @@
         <v>91</v>
       </c>
       <c r="D47" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E47" s="42"/>
       <c r="F47" s="43"/>
       <c r="G47" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H47" s="10">
         <v>45</v>
@@ -5071,20 +5069,20 @@
         <v>108</v>
       </c>
       <c r="J47" s="29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K47" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L47" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M47" s="23" t="s">
         <v>54</v>
       </c>
       <c r="N47" s="23"/>
       <c r="O47" s="30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P47" s="11" t="s">
         <v>19</v>
@@ -5099,13 +5097,13 @@
         <v>102</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U47" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:21">
       <c r="A48" s="15" t="s">
         <v>68</v>
       </c>
@@ -5116,12 +5114,12 @@
         <v>91</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E48" s="42"/>
       <c r="F48" s="43"/>
       <c r="G48" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H48" s="10">
         <v>46</v>
@@ -5130,39 +5128,39 @@
         <v>108</v>
       </c>
       <c r="J48" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K48" s="31" t="s">
         <v>70</v>
       </c>
       <c r="L48" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M48" s="23"/>
       <c r="N48" s="23"/>
       <c r="O48" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P48" s="11" t="s">
         <v>19</v>
       </c>
       <c r="Q48" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="R48" s="5" t="s">
         <v>97</v>
       </c>
       <c r="S48" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="U48" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.45">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
       <c r="A49" s="15" t="s">
         <v>68</v>
       </c>
@@ -5173,12 +5171,12 @@
         <v>91</v>
       </c>
       <c r="D49" s="44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E49" s="42"/>
       <c r="F49" s="43"/>
       <c r="G49" s="28" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H49" s="10">
         <v>47</v>
@@ -5187,7 +5185,7 @@
         <v>108</v>
       </c>
       <c r="J49" s="29" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K49" s="31" t="s">
         <v>69</v>
@@ -5207,7 +5205,7 @@
       <c r="T49" s="5"/>
       <c r="U49" s="33"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:21">
       <c r="A50" s="15" t="s">
         <v>68</v>
       </c>
@@ -5218,12 +5216,12 @@
         <v>91</v>
       </c>
       <c r="D50" s="44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E50" s="42"/>
       <c r="F50" s="43"/>
       <c r="G50" s="28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H50" s="10">
         <v>48</v>
@@ -5232,7 +5230,7 @@
         <v>108</v>
       </c>
       <c r="J50" s="29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K50" s="31" t="s">
         <v>69</v>
@@ -5245,7 +5243,7 @@
       </c>
       <c r="N50" s="23"/>
       <c r="O50" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P50" s="11" t="s">
         <v>19</v>
@@ -5260,13 +5258,13 @@
         <v>102</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="U50" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:21">
       <c r="A51" s="15" t="s">
         <v>68</v>
       </c>
@@ -5277,7 +5275,7 @@
         <v>91</v>
       </c>
       <c r="D51" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E51" s="42"/>
       <c r="F51" s="43"/>
@@ -5289,7 +5287,7 @@
         <v>108</v>
       </c>
       <c r="J51" s="29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K51" s="31" t="s">
         <v>69</v>
@@ -5302,7 +5300,7 @@
       </c>
       <c r="N51" s="23"/>
       <c r="O51" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P51" s="11" t="s">
         <v>20</v>
@@ -5317,13 +5315,13 @@
         <v>102</v>
       </c>
       <c r="T51" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="U51" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:21">
       <c r="A52" s="45"/>
       <c r="B52" s="46"/>
       <c r="C52" s="47"/>
@@ -5346,7 +5344,7 @@
       <c r="T52" s="5"/>
       <c r="U52" s="33"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:21">
       <c r="A53" s="45"/>
       <c r="B53" s="46"/>
       <c r="C53" s="47"/>
@@ -5369,7 +5367,7 @@
       <c r="T53" s="5"/>
       <c r="U53" s="33"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:21">
       <c r="A54" s="45"/>
       <c r="B54" s="46"/>
       <c r="C54" s="47"/>
@@ -5392,7 +5390,7 @@
       <c r="T54" s="5"/>
       <c r="U54" s="33"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:21">
       <c r="A55" s="45"/>
       <c r="B55" s="46"/>
       <c r="C55" s="47"/>
@@ -5415,7 +5413,7 @@
       <c r="T55" s="5"/>
       <c r="U55" s="33"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:21">
       <c r="A56" s="45"/>
       <c r="B56" s="46"/>
       <c r="C56" s="47"/>
@@ -5438,7 +5436,7 @@
       <c r="T56" s="5"/>
       <c r="U56" s="33"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:21">
       <c r="A57" s="45"/>
       <c r="B57" s="46"/>
       <c r="C57" s="47"/>
@@ -5461,7 +5459,7 @@
       <c r="T57" s="5"/>
       <c r="U57" s="33"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:21">
       <c r="A58" s="45"/>
       <c r="B58" s="46"/>
       <c r="C58" s="47"/>
@@ -5484,7 +5482,7 @@
       <c r="T58" s="5"/>
       <c r="U58" s="33"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:21">
       <c r="A59" s="45"/>
       <c r="B59" s="46"/>
       <c r="C59" s="47"/>
@@ -5507,7 +5505,7 @@
       <c r="T59" s="5"/>
       <c r="U59" s="33"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:21">
       <c r="A60" s="45"/>
       <c r="B60" s="46"/>
       <c r="C60" s="47"/>
@@ -5530,7 +5528,7 @@
       <c r="T60" s="5"/>
       <c r="U60" s="33"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:21">
       <c r="A61" s="45"/>
       <c r="B61" s="46"/>
       <c r="C61" s="47"/>
@@ -5553,7 +5551,7 @@
       <c r="T61" s="5"/>
       <c r="U61" s="33"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:21">
       <c r="A62" s="45"/>
       <c r="B62" s="46"/>
       <c r="C62" s="47"/>
@@ -5576,7 +5574,7 @@
       <c r="T62" s="5"/>
       <c r="U62" s="33"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:21">
       <c r="A63" s="45"/>
       <c r="B63" s="46"/>
       <c r="C63" s="47"/>
@@ -5599,7 +5597,7 @@
       <c r="T63" s="5"/>
       <c r="U63" s="33"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:21">
       <c r="A64" s="45"/>
       <c r="B64" s="46"/>
       <c r="C64" s="47"/>
@@ -5622,7 +5620,7 @@
       <c r="T64" s="5"/>
       <c r="U64" s="33"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:21">
       <c r="A65" s="45"/>
       <c r="B65" s="46"/>
       <c r="C65" s="47"/>
@@ -5645,7 +5643,7 @@
       <c r="T65" s="5"/>
       <c r="U65" s="33"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:21">
       <c r="A66" s="45"/>
       <c r="B66" s="46"/>
       <c r="C66" s="47"/>
@@ -5668,7 +5666,7 @@
       <c r="T66" s="5"/>
       <c r="U66" s="33"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:21">
       <c r="A67" s="45"/>
       <c r="B67" s="46"/>
       <c r="C67" s="47"/>
@@ -5691,7 +5689,7 @@
       <c r="T67" s="5"/>
       <c r="U67" s="33"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:21">
       <c r="A68" s="45"/>
       <c r="B68" s="46"/>
       <c r="C68" s="47"/>
@@ -5714,7 +5712,7 @@
       <c r="T68" s="5"/>
       <c r="U68" s="33"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:21">
       <c r="A69" s="45"/>
       <c r="B69" s="46"/>
       <c r="C69" s="47"/>
@@ -5737,7 +5735,7 @@
       <c r="T69" s="5"/>
       <c r="U69" s="33"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:21">
       <c r="A70" s="45"/>
       <c r="B70" s="46"/>
       <c r="C70" s="47"/>
@@ -5760,7 +5758,7 @@
       <c r="T70" s="5"/>
       <c r="U70" s="33"/>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:21">
       <c r="A71" s="45"/>
       <c r="B71" s="46"/>
       <c r="C71" s="47"/>
@@ -5783,7 +5781,7 @@
       <c r="T71" s="5"/>
       <c r="U71" s="33"/>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:21">
       <c r="A72" s="45"/>
       <c r="B72" s="46"/>
       <c r="C72" s="47"/>
@@ -5806,7 +5804,7 @@
       <c r="T72" s="5"/>
       <c r="U72" s="33"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:21">
       <c r="A73" s="45"/>
       <c r="B73" s="46"/>
       <c r="C73" s="47"/>
@@ -5829,7 +5827,7 @@
       <c r="T73" s="5"/>
       <c r="U73" s="33"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:21">
       <c r="A74" s="45"/>
       <c r="B74" s="46"/>
       <c r="C74" s="47"/>
@@ -5852,7 +5850,7 @@
       <c r="T74" s="5"/>
       <c r="U74" s="33"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:21">
       <c r="A75" s="45"/>
       <c r="B75" s="46"/>
       <c r="C75" s="47"/>
@@ -5875,7 +5873,7 @@
       <c r="T75" s="5"/>
       <c r="U75" s="33"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:21">
       <c r="A76" s="45"/>
       <c r="B76" s="46"/>
       <c r="C76" s="47"/>
@@ -5898,7 +5896,7 @@
       <c r="T76" s="5"/>
       <c r="U76" s="33"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:21">
       <c r="A77" s="45"/>
       <c r="B77" s="46"/>
       <c r="C77" s="47"/>
@@ -5921,7 +5919,7 @@
       <c r="T77" s="5"/>
       <c r="U77" s="33"/>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:21">
       <c r="A78" s="45"/>
       <c r="B78" s="46"/>
       <c r="C78" s="47"/>
@@ -5944,7 +5942,7 @@
       <c r="T78" s="5"/>
       <c r="U78" s="33"/>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:21">
       <c r="A79" s="45"/>
       <c r="B79" s="46"/>
       <c r="C79" s="47"/>
@@ -5967,7 +5965,7 @@
       <c r="T79" s="5"/>
       <c r="U79" s="33"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:21">
       <c r="A80" s="45"/>
       <c r="B80" s="46"/>
       <c r="C80" s="47"/>
@@ -5990,7 +5988,7 @@
       <c r="T80" s="5"/>
       <c r="U80" s="33"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:21">
       <c r="A81" s="45"/>
       <c r="B81" s="46"/>
       <c r="C81" s="47"/>
@@ -6013,7 +6011,7 @@
       <c r="T81" s="5"/>
       <c r="U81" s="33"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:21">
       <c r="A82" s="45"/>
       <c r="B82" s="46"/>
       <c r="C82" s="47"/>
@@ -6036,7 +6034,7 @@
       <c r="T82" s="5"/>
       <c r="U82" s="33"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:21">
       <c r="A83" s="45"/>
       <c r="B83" s="46"/>
       <c r="C83" s="47"/>
@@ -6059,7 +6057,7 @@
       <c r="T83" s="5"/>
       <c r="U83" s="33"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:21">
       <c r="A84" s="45"/>
       <c r="B84" s="46"/>
       <c r="C84" s="47"/>
@@ -6082,7 +6080,7 @@
       <c r="T84" s="5"/>
       <c r="U84" s="33"/>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:21">
       <c r="A85" s="45"/>
       <c r="B85" s="46"/>
       <c r="C85" s="47"/>
@@ -6105,7 +6103,7 @@
       <c r="T85" s="5"/>
       <c r="U85" s="33"/>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:21">
       <c r="A86" s="45"/>
       <c r="B86" s="46"/>
       <c r="C86" s="47"/>
@@ -6128,7 +6126,7 @@
       <c r="T86" s="5"/>
       <c r="U86" s="33"/>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:21">
       <c r="A87" s="45"/>
       <c r="B87" s="46"/>
       <c r="C87" s="47"/>
@@ -6151,7 +6149,7 @@
       <c r="T87" s="5"/>
       <c r="U87" s="33"/>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:21">
       <c r="A88" s="45"/>
       <c r="B88" s="46"/>
       <c r="C88" s="47"/>
@@ -6174,7 +6172,7 @@
       <c r="T88" s="5"/>
       <c r="U88" s="33"/>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:21">
       <c r="A89" s="45"/>
       <c r="B89" s="46"/>
       <c r="C89" s="47"/>
@@ -6197,7 +6195,7 @@
       <c r="T89" s="5"/>
       <c r="U89" s="33"/>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:21">
       <c r="A90" s="45"/>
       <c r="B90" s="46"/>
       <c r="C90" s="47"/>
@@ -6220,7 +6218,7 @@
       <c r="T90" s="5"/>
       <c r="U90" s="33"/>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:21">
       <c r="A91" s="45"/>
       <c r="B91" s="46"/>
       <c r="C91" s="47"/>
@@ -6248,11 +6246,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -6268,9 +6261,13 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6281,23 +6278,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2"/>
+  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="14.46484375" customWidth="1"/>
-    <col min="4" max="4" width="13.796875" customWidth="1"/>
-    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -6320,7 +6317,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
         <v>34</v>
@@ -6341,7 +6338,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>35</v>
@@ -6362,7 +6359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>36</v>
@@ -6379,7 +6376,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>37</v>
@@ -6396,7 +6393,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
         <v>38</v>
@@ -6411,7 +6408,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
         <v>39</v>
@@ -6424,7 +6421,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
         <v>40</v>
@@ -6437,7 +6434,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
         <v>41</v>
@@ -6450,7 +6447,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14">
       <c r="A10" s="7"/>
       <c r="B10" s="7" t="s">
         <v>42</v>
@@ -6463,7 +6460,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14">
       <c r="A11" s="7"/>
       <c r="B11" s="7" t="s">
         <v>43</v>
@@ -6478,7 +6475,7 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14">
       <c r="A12" s="7"/>
       <c r="B12" s="7" t="s">
         <v>44</v>
@@ -6493,7 +6490,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
         <v>45</v>
@@ -6508,7 +6505,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14">
       <c r="A14" s="7"/>
       <c r="B14" s="7" t="s">
         <v>46</v>
@@ -6523,7 +6520,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
@@ -6536,7 +6533,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
@@ -6549,7 +6546,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
@@ -6562,7 +6559,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
@@ -6575,7 +6572,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
@@ -6588,7 +6585,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
@@ -6601,7 +6598,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
@@ -6614,7 +6611,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
@@ -6627,7 +6624,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
@@ -6640,7 +6637,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
@@ -6653,7 +6650,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
@@ -6664,7 +6661,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
@@ -6675,7 +6672,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
@@ -6686,7 +6683,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
@@ -6697,7 +6694,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
@@ -6708,7 +6705,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7" t="s">
@@ -6719,7 +6716,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
@@ -6730,7 +6727,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
@@ -6741,7 +6738,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7" t="s">
@@ -6752,7 +6749,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
@@ -6763,7 +6760,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
@@ -6774,7 +6771,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7" t="s">
@@ -6785,7 +6782,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="7" t="s">
@@ -6796,7 +6793,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4" t="s">
@@ -6807,7 +6804,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
@@ -6818,7 +6815,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -6827,7 +6824,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -6836,7 +6833,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -6845,7 +6842,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -6854,7 +6851,7 @@
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -6863,7 +6860,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -6872,7 +6869,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -6881,7 +6878,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -6890,7 +6887,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -6899,7 +6896,7 @@
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -6908,7 +6905,7 @@
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>

</xml_diff>